<commit_message>
1.4 add a condition
</commit_message>
<xml_diff>
--- a/模板9.8.xlsx
+++ b/模板9.8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\sssimonyang\projects\stock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9327874A-392E-43FD-89FE-3D1E72659117}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C2029C3-89F3-4024-9FB7-98BCB0E4A74D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>9点35分前有上万白单，全天无大于10001的卖单或者卖单</t>
   </si>
@@ -60,6 +60,10 @@
   </si>
   <si>
     <t>9点40分前有上千白单，全天无901以上买单或者卖单</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>9点40分钱有白单（大于10），9点40分前无101以上买单或者卖单，10点前无101以上卖单，且全天无901以上买单或者卖单</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -449,9 +453,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.88671875" customWidth="1"/>
-    <col min="2" max="5" width="21.6640625" customWidth="1"/>
-    <col min="6" max="6" width="48" customWidth="1"/>
+    <col min="1" max="6" width="19.88671875" customWidth="1"/>
+    <col min="7" max="7" width="35.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="108" customHeight="1" x14ac:dyDescent="0.25">
@@ -467,7 +470,10 @@
       <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -476,33 +482,30 @@
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="3"/>
+      <c r="G3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="4"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="3"/>
+      <c r="G4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>

</xml_diff>